<commit_message>
Describe your changes to Demo_Odoo.py
</commit_message>
<xml_diff>
--- a/analisis_2025.xlsx
+++ b/analisis_2025.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego Mauricio\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego Mauricio\Desktop\FERREINOX VENTAS\Resumen-Ventas-Gerenciales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6BD4EF55-493A-472B-A6EF-891946DAC50F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF94A1AD-B947-42AA-9C1E-A07F3F4BEA21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{63AEA62F-EC17-43D5-AF0F-9EF4AE21A00F}"/>
   </bookViews>
@@ -539,8 +539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25A163E6-1D09-4EB4-8232-A18C2DC2CE08}">
   <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="30.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -668,14 +668,14 @@
         <v>8</v>
       </c>
       <c r="B3" s="5">
-        <v>112316688.87530416</v>
+        <v>3000000000</v>
       </c>
       <c r="C3" s="5">
         <v>85124421.748069391</v>
       </c>
       <c r="D3" s="6">
         <f t="shared" si="0"/>
-        <v>0.31944143136398445</v>
+        <v>34.242530150497494</v>
       </c>
       <c r="E3" s="7">
         <v>0</v>
@@ -699,14 +699,14 @@
         <v>9</v>
       </c>
       <c r="B4" s="5">
-        <v>1574862189.7271142</v>
+        <v>1574862189.7271099</v>
       </c>
       <c r="C4" s="5">
         <v>1302400689.8146079</v>
       </c>
       <c r="D4" s="6">
         <f t="shared" si="0"/>
-        <v>0.20919944379888977</v>
+        <v>0.2091994437988865</v>
       </c>
       <c r="E4" s="7">
         <v>16</v>

</xml_diff>